<commit_message>
account sign up not verify DOING..
</commit_message>
<xml_diff>
--- a/FSANDROID/TestSuite/Android/Data.xlsx
+++ b/FSANDROID/TestSuite/Android/Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>sta</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>sta25.115@yopmail.com</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>expected xuong dong thi anh xu ly theo cach xuong dong (replace '\n' by '${EMPTY}')</t>
   </si>
 </sst>
 </file>
@@ -382,29 +388,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="84" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="78.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>25.1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -412,7 +425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1234</v>
       </c>
@@ -420,7 +433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -428,7 +441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>